<commit_message>
Fix flow when a new bow model is created
</commit_message>
<xml_diff>
--- a/test_sample_data/true/registers_2020-03-09_13.xlsx
+++ b/test_sample_data/true/registers_2020-03-09_13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15580" activeTab="4"/>
+    <workbookView windowHeight="16820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -1267,12 +1267,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1371,8 +1371,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1385,8 +1386,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -1403,38 +1435,65 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1448,68 +1507,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1530,19 +1530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1554,43 +1542,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1602,55 +1578,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1668,13 +1596,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1686,31 +1680,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1739,26 +1739,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1787,6 +1787,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1804,180 +1815,169 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1986,7 +1986,7 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2015,7 +2015,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2312,7 +2312,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12:N16"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -2618,7 +2618,6 @@
       <c r="K9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L9"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -2777,11 +2776,11 @@
         <v>0</v>
       </c>
       <c r="M13" s="22">
-        <v>50.96</v>
+        <v>48.47</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" ref="N13:N16" si="0">ABS(L13-M13)</f>
-        <v>50.96</v>
+        <v>48.47</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2825,11 +2824,11 @@
         <v>0</v>
       </c>
       <c r="M14" s="22">
-        <v>20.01</v>
+        <v>18.37</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>20.01</v>
+        <v>18.37</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2873,11 +2872,11 @@
         <v>0</v>
       </c>
       <c r="M15" s="22">
-        <v>4.14</v>
+        <v>2.48</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>4.14</v>
+        <v>2.48</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -2921,11 +2920,11 @@
         <v>0</v>
       </c>
       <c r="M16" s="22">
-        <v>4.49</v>
+        <v>3.66</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="0"/>
-        <v>4.49</v>
+        <v>3.66</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -2957,7 +2956,7 @@
         <v>32</v>
       </c>
       <c r="J17" s="19">
-        <f t="shared" ref="J17:L17" si="1">SUM(J13:J16)</f>
+        <f t="shared" ref="J17:N17" si="1">SUM(J13:J16)</f>
         <v>152</v>
       </c>
       <c r="K17" s="19">
@@ -2969,12 +2968,12 @@
         <v>0</v>
       </c>
       <c r="M17" s="23">
-        <f>SUM(M13:M16)</f>
-        <v>79.6</v>
+        <f t="shared" si="1"/>
+        <v>72.98</v>
       </c>
       <c r="N17" s="20">
-        <f>SUM(N13:N16)</f>
-        <v>79.6</v>
+        <f t="shared" si="1"/>
+        <v>72.98</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -9850,7 +9849,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12:N16"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -10150,7 +10149,6 @@
       <c r="K9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L9"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -10307,11 +10305,11 @@
         <v>90</v>
       </c>
       <c r="M13" s="22">
-        <v>79.56</v>
+        <v>85.89</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" ref="N13:N16" si="0">ABS(L13-M13)</f>
-        <v>10.44</v>
+        <v>4.11</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -10355,11 +10353,11 @@
         <v>30</v>
       </c>
       <c r="M14" s="22">
-        <v>19.68</v>
+        <v>19.56</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>10.32</v>
+        <v>10.44</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -10401,11 +10399,11 @@
         <v>3</v>
       </c>
       <c r="M15" s="22">
-        <v>4.14</v>
+        <v>2.94</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>1.14</v>
+        <v>0.0600000000000001</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -10447,11 +10445,11 @@
         <v>19</v>
       </c>
       <c r="M16" s="22">
-        <v>15.52</v>
+        <v>15.3</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="0"/>
-        <v>3.48</v>
+        <v>3.7</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -10496,11 +10494,11 @@
       </c>
       <c r="M17" s="23">
         <f t="shared" si="1"/>
-        <v>118.9</v>
+        <v>123.69</v>
       </c>
       <c r="N17" s="20">
         <f t="shared" si="1"/>
-        <v>25.38</v>
+        <v>18.31</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -21612,7 +21610,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12:N16"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -21912,7 +21910,6 @@
       <c r="K9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L9"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -22069,11 +22066,11 @@
         <v>93</v>
       </c>
       <c r="M13" s="22">
-        <v>79.56</v>
+        <v>86.3</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" ref="N13:N16" si="0">ABS(L13-M13)</f>
-        <v>13.44</v>
+        <v>6.7</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -22117,11 +22114,11 @@
         <v>26</v>
       </c>
       <c r="M14" s="22">
-        <v>19.68</v>
+        <v>19.97</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>6.32</v>
+        <v>6.03</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -22163,11 +22160,11 @@
         <v>2</v>
       </c>
       <c r="M15" s="22">
-        <v>2.58</v>
+        <v>2.48</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>0.58</v>
+        <v>0.48</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -22209,11 +22206,11 @@
         <v>18</v>
       </c>
       <c r="M16" s="22">
-        <v>13.96</v>
+        <v>15.71</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="0"/>
-        <v>4.04</v>
+        <v>2.29</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -22258,11 +22255,11 @@
       </c>
       <c r="M17" s="23">
         <f t="shared" si="1"/>
-        <v>115.78</v>
+        <v>124.46</v>
       </c>
       <c r="N17" s="20">
         <f t="shared" si="1"/>
-        <v>24.38</v>
+        <v>15.5</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -33204,7 +33201,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12:N16"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -33504,7 +33501,6 @@
       <c r="K9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L9"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -33661,11 +33657,11 @@
         <v>88</v>
       </c>
       <c r="M13" s="22">
-        <v>83.47</v>
+        <v>86.58</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" ref="N13:N16" si="0">ABS(L13-M13)</f>
-        <v>4.53</v>
+        <v>1.42</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -33709,11 +33705,11 @@
         <v>23</v>
       </c>
       <c r="M14" s="22">
-        <v>16.1</v>
+        <v>17.28</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>6.9</v>
+        <v>5.72</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -33755,11 +33751,11 @@
         <v>4</v>
       </c>
       <c r="M15" s="22">
-        <v>4.14</v>
+        <v>2.94</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>0.14</v>
+        <v>1.06</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -33801,11 +33797,11 @@
         <v>19</v>
       </c>
       <c r="M16" s="22">
-        <v>16.1</v>
+        <v>17.28</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="0"/>
-        <v>2.9</v>
+        <v>1.72</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -33850,11 +33846,11 @@
       </c>
       <c r="M17" s="23">
         <f t="shared" si="1"/>
-        <v>119.81</v>
+        <v>124.08</v>
       </c>
       <c r="N17" s="20">
         <f t="shared" si="1"/>
-        <v>14.47</v>
+        <v>9.92</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -44576,7 +44572,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -44619,7 +44615,6 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -45044,11 +45039,11 @@
         <v>125</v>
       </c>
       <c r="M13" s="22">
-        <v>82.71</v>
+        <v>92.32</v>
       </c>
       <c r="N13" s="18">
         <f>ABS(L13-M13)</f>
-        <v>42.29</v>
+        <v>32.68</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -45092,11 +45087,11 @@
         <v>14</v>
       </c>
       <c r="M14" s="22">
-        <v>11.64</v>
+        <v>11.05</v>
       </c>
       <c r="N14" s="18">
         <f>ABS(L14-M14)</f>
-        <v>2.36</v>
+        <v>2.95</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -45138,11 +45133,11 @@
         <v>2</v>
       </c>
       <c r="M15" s="22">
-        <v>4.14</v>
+        <v>2.94</v>
       </c>
       <c r="N15" s="18">
         <f>ABS(L15-M15)</f>
-        <v>2.14</v>
+        <v>0.94</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -45184,11 +45179,11 @@
         <v>13</v>
       </c>
       <c r="M16" s="22">
-        <v>11.64</v>
+        <v>11.05</v>
       </c>
       <c r="N16" s="18">
         <f>ABS(L16-M16)</f>
-        <v>1.36</v>
+        <v>1.95</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -45233,11 +45228,11 @@
       </c>
       <c r="M17" s="23">
         <f>SUM(M13:M16)</f>
-        <v>110.13</v>
+        <v>117.36</v>
       </c>
       <c r="N17" s="20">
         <f>SUM(N13:N16)</f>
-        <v>48.15</v>
+        <v>38.52</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -45360,7 +45355,6 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="12"/>
-      <c r="L21"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>

</xml_diff>